<commit_message>
More work in progress on auto regression tests.
</commit_message>
<xml_diff>
--- a/src/Tests/RegressionTests/Expected/Formulae.xlsx
+++ b/src/Tests/RegressionTests/Expected/Formulae.xlsx
@@ -44,7 +44,7 @@
   <x:numFmts count="4">
     <x:numFmt numFmtId="0" formatCode=""/>
     <x:numFmt numFmtId="165" formatCode="$0.00"/>
-    <x:numFmt numFmtId="166" formatCode="#,###"/>
+    <x:numFmt numFmtId="166" formatCode="#,##0"/>
     <x:numFmt numFmtId="167" formatCode="$#,##0.00"/>
   </x:numFmts>
   <x:fonts count="2">
@@ -471,10 +471,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="3" t="n">
-        <x:v>573.807582672949</x:v>
+        <x:v>141.5</x:v>
       </x:c>
       <x:c r="C2" s="4" t="n">
-        <x:v>62</x:v>
+        <x:v>926</x:v>
       </x:c>
       <x:c r="D2" s="5">
         <x:f>B2*C2</x:f>
@@ -485,10 +485,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B3" s="3" t="n">
-        <x:v>638.692999143661</x:v>
+        <x:v>0.314</x:v>
       </x:c>
       <x:c r="C3" s="4" t="n">
-        <x:v>86</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="D3" s="5">
         <x:f>B3*C3</x:f>
@@ -499,10 +499,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="3" t="n">
-        <x:v>91.2616170447892</x:v>
+        <x:v>653.5</x:v>
       </x:c>
       <x:c r="C4" s="4" t="n">
-        <x:v>29</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D4" s="5">
         <x:f>B4*C4</x:f>

</xml_diff>

<commit_message>
Improve random number generator.
</commit_message>
<xml_diff>
--- a/src/Tests/RegressionTests/Expected/Formulae.xlsx
+++ b/src/Tests/RegressionTests/Expected/Formulae.xlsx
@@ -471,10 +471,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="3" t="n">
-        <x:v>141.5</x:v>
+        <x:v>0.022477936010099</x:v>
       </x:c>
       <x:c r="C2" s="4" t="n">
-        <x:v>926</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="D2" s="5">
         <x:f>B2*C2</x:f>
@@ -485,10 +485,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B3" s="3" t="n">
-        <x:v>0.314</x:v>
+        <x:v>601.352605317418</x:v>
       </x:c>
       <x:c r="C3" s="4" t="n">
-        <x:v>159</x:v>
+        <x:v>891</x:v>
       </x:c>
       <x:c r="D3" s="5">
         <x:f>B3*C3</x:f>
@@ -499,10 +499,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="3" t="n">
-        <x:v>653.5</x:v>
+        <x:v>967.955701969543</x:v>
       </x:c>
       <x:c r="C4" s="4" t="n">
-        <x:v>141</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="D4" s="5">
         <x:f>B4*C4</x:f>

</xml_diff>